<commit_message>
web 120 / Homework 02
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7BD8F0-764B-43A0-8CC6-D1371FB1255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3436CE-E946-43AC-AE4E-B0C9E2931145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>No.</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Q01</t>
+  </si>
+  <si>
+    <t>H02</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,9 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -622,7 +627,9 @@
       <c r="B2" s="13">
         <v>5</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="13">
+        <v>9</v>
+      </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -645,7 +652,9 @@
       <c r="B3" s="13">
         <v>7</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="13">
+        <v>9.5</v>
+      </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -668,7 +677,9 @@
       <c r="B4" s="13">
         <v>8</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="13">
+        <v>6</v>
+      </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -689,7 +700,9 @@
       <c r="B5" s="13">
         <v>8</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -710,7 +723,9 @@
       <c r="B6" s="13">
         <v>9</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="13">
+        <v>10</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -731,7 +746,9 @@
       <c r="B7" s="4">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -752,7 +769,9 @@
       <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -773,7 +792,9 @@
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4">
+        <v>10</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -794,9 +815,11 @@
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -814,6 +837,9 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
+      <c r="C11" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -822,6 +848,9 @@
       <c r="B12" s="4">
         <v>6</v>
       </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -830,6 +859,9 @@
       <c r="B13" s="4">
         <v>6</v>
       </c>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -838,6 +870,9 @@
       <c r="B14" s="4">
         <v>5</v>
       </c>
+      <c r="C14" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -846,6 +881,9 @@
       <c r="B15" s="4">
         <v>4</v>
       </c>
+      <c r="C15" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -854,14 +892,17 @@
       <c r="B16" s="4">
         <v>7</v>
       </c>
+      <c r="C16" s="4">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="7">
-        <f>COUNTA(B1) * 10</f>
-        <v>10</v>
+        <f>COUNTA(B1:Q1) * 10</f>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,8 +935,8 @@
         <v>1</v>
       </c>
       <c r="B22" s="10">
-        <f>(SUM(B2)/B17) * 40</f>
-        <v>20</v>
+        <f>(SUM(B2:R2)/B17) * 40</f>
+        <v>28</v>
       </c>
       <c r="C22" s="11">
         <v>0</v>
@@ -905,11 +946,11 @@
       </c>
       <c r="E22" s="12">
         <f>B22+C22+D22</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F22" s="15">
         <f>E22</f>
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -917,8 +958,8 @@
         <v>2</v>
       </c>
       <c r="B23" s="10">
-        <f>(SUM(B3)/B17) * 40</f>
-        <v>28</v>
+        <f>(SUM(B3:R3)/B17) * 40</f>
+        <v>33</v>
       </c>
       <c r="C23" s="11">
         <v>0</v>
@@ -928,11 +969,11 @@
       </c>
       <c r="E23" s="12">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,8 +981,8 @@
         <v>3</v>
       </c>
       <c r="B24" s="10">
-        <f>(SUM(B4)/B17) * 40</f>
-        <v>32</v>
+        <f>(SUM(B4:R4)/B17) * 40</f>
+        <v>28</v>
       </c>
       <c r="C24" s="11">
         <v>0</v>
@@ -951,11 +992,11 @@
       </c>
       <c r="E24" s="12">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -963,8 +1004,8 @@
         <v>4</v>
       </c>
       <c r="B25" s="10">
-        <f>(SUM(B5)/B17) * 40</f>
-        <v>32</v>
+        <f>(SUM(B5:R5)/B17) * 40</f>
+        <v>16</v>
       </c>
       <c r="C25" s="11">
         <v>0</v>
@@ -974,11 +1015,11 @@
       </c>
       <c r="E25" s="12">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -986,8 +1027,8 @@
         <v>5</v>
       </c>
       <c r="B26" s="10">
-        <f>(SUM(B6)/B17) * 40</f>
-        <v>36</v>
+        <f>(SUM(B6:R6)/B17) * 40</f>
+        <v>38</v>
       </c>
       <c r="C26" s="11">
         <v>0</v>
@@ -997,11 +1038,11 @@
       </c>
       <c r="E26" s="12">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1009,8 +1050,8 @@
         <v>6</v>
       </c>
       <c r="B27" s="10">
-        <f>(SUM(B7)/B17) * 40</f>
-        <v>40</v>
+        <f>(SUM(B7:R7)/B17) * 40</f>
+        <v>20</v>
       </c>
       <c r="C27" s="11">
         <v>0</v>
@@ -1020,11 +1061,11 @@
       </c>
       <c r="E27" s="12">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,7 +1073,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="10">
-        <f>(SUM(B8)/B17) * 40</f>
+        <f>(SUM(B8:R8)/B17) * 40</f>
         <v>0</v>
       </c>
       <c r="C28" s="11">
@@ -1055,8 +1096,8 @@
         <v>8</v>
       </c>
       <c r="B29" s="10">
-        <f>(SUM(B9)/B17) * 40</f>
-        <v>28</v>
+        <f>(SUM(B9:R9)/B17) * 40</f>
+        <v>34</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -1066,11 +1107,11 @@
       </c>
       <c r="E29" s="12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,8 +1119,8 @@
         <v>9</v>
       </c>
       <c r="B30" s="10">
-        <f>(SUM(B10)/B17) * 40</f>
-        <v>12</v>
+        <f>(SUM(B10:R10)/B17) * 40</f>
+        <v>25</v>
       </c>
       <c r="C30" s="11">
         <v>0</v>
@@ -1089,11 +1130,11 @@
       </c>
       <c r="E30" s="12">
         <f>B30+C30+D30</f>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="10">
-        <f>(SUM(B11)/B17) * 40</f>
+        <f>(SUM(B11:R11)/B17) * 40</f>
         <v>28</v>
       </c>
       <c r="C31" s="11">
@@ -1124,8 +1165,8 @@
         <v>11</v>
       </c>
       <c r="B32" s="10">
-        <f>(SUM(B12)/B17) * 40</f>
-        <v>24</v>
+        <f>(SUM(B12:R12)/B17) * 40</f>
+        <v>32</v>
       </c>
       <c r="C32" s="11">
         <v>0</v>
@@ -1135,11 +1176,11 @@
       </c>
       <c r="E32" s="12">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1147,8 +1188,8 @@
         <v>12</v>
       </c>
       <c r="B33" s="10">
-        <f>(SUM(B13)/B17) * 40</f>
-        <v>24</v>
+        <f>(SUM(B13:R13)/B17) * 40</f>
+        <v>22</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
@@ -1158,11 +1199,11 @@
       </c>
       <c r="E33" s="12">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,8 +1211,8 @@
         <v>13</v>
       </c>
       <c r="B34" s="10">
-        <f>(SUM(B14)/B17) * 40</f>
-        <v>20</v>
+        <f>(SUM(B14:R14)/B17) * 40</f>
+        <v>24</v>
       </c>
       <c r="C34" s="11">
         <v>0</v>
@@ -1181,11 +1222,11 @@
       </c>
       <c r="E34" s="12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,8 +1234,8 @@
         <v>14</v>
       </c>
       <c r="B35" s="10">
-        <f>(SUM(B15)/B17) * 40</f>
-        <v>16</v>
+        <f>(SUM(B15:R15)/B17) * 40</f>
+        <v>28</v>
       </c>
       <c r="C35" s="11">
         <v>0</v>
@@ -1204,11 +1245,11 @@
       </c>
       <c r="E35" s="12">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,8 +1257,8 @@
         <v>15</v>
       </c>
       <c r="B36" s="10">
-        <f>(SUM(B16)/B17) * 40</f>
-        <v>28</v>
+        <f>(SUM(B16:R16)/B17) * 40</f>
+        <v>31</v>
       </c>
       <c r="C36" s="11">
         <v>0</v>
@@ -1227,11 +1268,11 @@
       </c>
       <c r="E36" s="12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 120 / Homework 03 & Homework 05
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3436CE-E946-43AC-AE4E-B0C9E2931145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568EDD3D-E485-4F24-B67B-B6D5F5B2E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>No.</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>H02</t>
+  </si>
+  <si>
+    <t>H03</t>
+  </si>
+  <si>
+    <t>H05</t>
   </si>
 </sst>
 </file>
@@ -83,7 +89,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +138,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +199,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +593,7 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,8 +623,12 @@
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -630,8 +652,12 @@
       <c r="C2" s="13">
         <v>9</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="13">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <v>9.5</v>
+      </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -655,8 +681,12 @@
       <c r="C3" s="13">
         <v>9.5</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="13">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13">
+        <v>10</v>
+      </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -680,8 +710,12 @@
       <c r="C4" s="13">
         <v>6</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="13">
+        <v>7</v>
+      </c>
+      <c r="E4" s="13">
+        <v>8.5</v>
+      </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -703,8 +737,12 @@
       <c r="C5" s="13">
         <v>0</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>9</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -726,8 +764,12 @@
       <c r="C6" s="13">
         <v>10</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="13">
+        <v>9.75</v>
+      </c>
+      <c r="E6" s="13">
+        <v>10</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -747,10 +789,14 @@
         <v>10</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>9</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -772,8 +818,12 @@
       <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -795,8 +845,12 @@
       <c r="C9" s="4">
         <v>10</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
+        <v>9.75</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -818,8 +872,12 @@
       <c r="C10" s="4">
         <v>9.5</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -840,6 +898,12 @@
       <c r="C11" s="4">
         <v>7</v>
       </c>
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -851,6 +915,12 @@
       <c r="C12" s="4">
         <v>10</v>
       </c>
+      <c r="D12" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -862,6 +932,13 @@
       <c r="C13" s="4">
         <v>5</v>
       </c>
+      <c r="D13" s="19">
+        <f>9.5/2</f>
+        <v>4.75</v>
+      </c>
+      <c r="E13" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -873,6 +950,12 @@
       <c r="C14" s="4">
         <v>7</v>
       </c>
+      <c r="D14" s="4">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.5</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -884,6 +967,13 @@
       <c r="C15" s="4">
         <v>10</v>
       </c>
+      <c r="D15" s="20">
+        <f>10/2</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -895,6 +985,12 @@
       <c r="C16" s="4">
         <v>8.5</v>
       </c>
+      <c r="D16" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -902,7 +998,7 @@
       </c>
       <c r="B17" s="7">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,7 +1032,7 @@
       </c>
       <c r="B22" s="10">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>28</v>
+        <v>33.5</v>
       </c>
       <c r="C22" s="11">
         <v>0</v>
@@ -946,11 +1042,11 @@
       </c>
       <c r="E22" s="12">
         <f>B22+C22+D22</f>
-        <v>28</v>
+        <v>33.5</v>
       </c>
       <c r="F22" s="15">
         <f>E22</f>
-        <v>28</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,21 +1055,21 @@
       </c>
       <c r="B23" s="10">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>33</v>
+        <v>36.5</v>
       </c>
       <c r="C23" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="11">
         <v>0</v>
       </c>
       <c r="E23" s="12">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>33</v>
+        <v>37.5</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>33</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,7 +1078,7 @@
       </c>
       <c r="B24" s="10">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>28</v>
+        <v>29.5</v>
       </c>
       <c r="C24" s="11">
         <v>0</v>
@@ -992,11 +1088,11 @@
       </c>
       <c r="E24" s="12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29.5</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,7 +1101,7 @@
       </c>
       <c r="B25" s="10">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="11">
         <v>0</v>
@@ -1015,11 +1111,11 @@
       </c>
       <c r="E25" s="12">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,21 +1124,21 @@
       </c>
       <c r="B26" s="10">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>38</v>
+        <v>38.75</v>
       </c>
       <c r="C26" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="11">
         <v>0</v>
       </c>
       <c r="E26" s="12">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39.75</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,7 +1147,7 @@
       </c>
       <c r="B27" s="10">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>20</v>
+        <v>35.5</v>
       </c>
       <c r="C27" s="11">
         <v>0</v>
@@ -1061,11 +1157,11 @@
       </c>
       <c r="E27" s="12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>35.5</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1097,21 +1193,21 @@
       </c>
       <c r="B29" s="10">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>34</v>
+        <v>36.75</v>
       </c>
       <c r="C29" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="11">
         <v>0</v>
       </c>
       <c r="E29" s="12">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>37.75</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>37.75</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,7 +1216,7 @@
       </c>
       <c r="B30" s="10">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>25</v>
+        <v>30.5</v>
       </c>
       <c r="C30" s="11">
         <v>0</v>
@@ -1130,11 +1226,11 @@
       </c>
       <c r="E30" s="12">
         <f>B30+C30+D30</f>
-        <v>25</v>
+        <v>30.5</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1143,21 +1239,21 @@
       </c>
       <c r="B31" s="10">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="11">
         <v>0</v>
       </c>
       <c r="E31" s="12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1166,7 +1262,7 @@
       </c>
       <c r="B32" s="10">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C32" s="11">
         <v>0</v>
@@ -1176,11 +1272,11 @@
       </c>
       <c r="E32" s="12">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1189,7 +1285,7 @@
       </c>
       <c r="B33" s="10">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>22</v>
+        <v>25.75</v>
       </c>
       <c r="C33" s="11">
         <v>0</v>
@@ -1199,11 +1295,11 @@
       </c>
       <c r="E33" s="12">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25.75</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>25.75</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1308,7 @@
       </c>
       <c r="B34" s="10">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>24</v>
+        <v>25.5</v>
       </c>
       <c r="C34" s="11">
         <v>0</v>
@@ -1222,11 +1318,11 @@
       </c>
       <c r="E34" s="12">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25.5</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,7 +1331,7 @@
       </c>
       <c r="B35" s="10">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C35" s="11">
         <v>0</v>
@@ -1245,11 +1341,11 @@
       </c>
       <c r="E35" s="12">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,7 +1354,7 @@
       </c>
       <c r="B36" s="10">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C36" s="11">
         <v>0</v>
@@ -1268,11 +1364,11 @@
       </c>
       <c r="E36" s="12">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 120 / Session 06
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6C4F6-1D32-42B8-9CB2-6331C0D1E76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79666CBD-AFC5-4B2E-B96E-9229729AACCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Q02</t>
+  </si>
+  <si>
+    <t>H06</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +599,7 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
@@ -624,7 +627,9 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -656,7 +661,9 @@
         <f>(10/12)*10</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="15">
+        <v>11</v>
+      </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -697,7 +704,9 @@
         <f>(12/12)*10</f>
         <v>10</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15">
+        <v>10</v>
+      </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -738,7 +747,9 @@
         <f>(9/12)*10</f>
         <v>7.5</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="15">
+        <v>9.75</v>
+      </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -767,10 +778,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5" s="15">
         <v>9</v>
@@ -779,7 +790,9 @@
         <f>(7/12)*10</f>
         <v>5.8333333333333339</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="15">
+        <v>8.5</v>
+      </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -820,7 +833,9 @@
         <f>(12/12)*10</f>
         <v>10</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="15">
+        <v>9.75</v>
+      </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -861,7 +876,9 @@
         <f>(11/12)*10</f>
         <v>9.1666666666666661</v>
       </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17">
+        <v>9</v>
+      </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -901,7 +918,9 @@
       <c r="F8" s="17">
         <v>0</v>
       </c>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17">
+        <v>0</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -942,7 +961,9 @@
         <f>(12/12)*10</f>
         <v>10</v>
       </c>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17">
+        <v>10.5</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
@@ -980,10 +1001,12 @@
         <v>8</v>
       </c>
       <c r="F10" s="17">
-        <f>(10/12)*10</f>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="G10" s="17"/>
+        <f>(11/12)*10</f>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="G10" s="17">
+        <v>6.5</v>
+      </c>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -1024,7 +1047,9 @@
         <f>(5/12)*10</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="17">
+        <v>8</v>
+      </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
@@ -1065,7 +1090,9 @@
         <f>(6/12)*10</f>
         <v>5</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="17">
+        <v>10.5</v>
+      </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
@@ -1106,7 +1133,9 @@
         <f>(10/12)*10</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="17">
+        <v>9</v>
+      </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="17"/>
@@ -1147,7 +1176,9 @@
         <f>(6/12)*10</f>
         <v>5</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="17"/>
@@ -1188,7 +1219,9 @@
       <c r="F15" s="17">
         <v>0</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="17">
+        <v>9.75</v>
+      </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="17"/>
@@ -1229,7 +1262,9 @@
         <f>(11/12)*10</f>
         <v>9.1666666666666661</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="17">
+        <v>9</v>
+      </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
       <c r="J16" s="17"/>
@@ -1256,13 +1291,13 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
@@ -1314,7 +1349,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>33.466666666666669</v>
+        <v>35.222222222222229</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1324,11 +1359,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>33.466666666666669</v>
+        <v>35.222222222222229</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>33.466666666666669</v>
+        <v>35.222222222222229</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1337,7 +1372,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>37.200000000000003</v>
+        <v>37.666666666666664</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1347,11 +1382,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>38.200000000000003</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>38.200000000000003</v>
+        <v>38.666666666666664</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1360,7 +1395,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>29.6</v>
+        <v>31.166666666666668</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1370,11 +1405,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>29.6</v>
+        <v>31.166666666666668</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>29.6</v>
+        <v>31.166666666666668</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1383,7 +1418,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>18.266666666666669</v>
+        <v>30.222222222222225</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1393,11 +1428,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>18.266666666666669</v>
+        <v>30.222222222222225</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>18.266666666666669</v>
+        <v>30.222222222222225</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1429,7 +1464,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>35.733333333333334</v>
+        <v>35.777777777777771</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1439,11 +1474,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>35.733333333333334</v>
+        <v>35.777777777777771</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>35.733333333333334</v>
+        <v>35.777777777777771</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1475,7 +1510,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>37.400000000000006</v>
+        <v>38.166666666666671</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1485,11 +1520,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>38.400000000000006</v>
+        <v>39.166666666666671</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>38.400000000000006</v>
+        <v>39.166666666666671</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1498,7 +1533,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>31.06666666666667</v>
+        <v>30.777777777777775</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1508,11 +1543,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>31.06666666666667</v>
+        <v>30.777777777777775</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>31.06666666666667</v>
+        <v>30.777777777777775</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1521,7 +1556,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>27.333333333333329</v>
+        <v>28.111111111111107</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1531,11 +1566,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>28.333333333333329</v>
+        <v>29.111111111111107</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>28.333333333333329</v>
+        <v>29.111111111111107</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1544,7 +1579,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>32</v>
+        <v>33.666666666666664</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1554,11 +1589,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33.666666666666664</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33.666666666666664</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,7 +1602,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>31.06666666666667</v>
+        <v>31.888888888888893</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1577,11 +1612,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>31.06666666666667</v>
+        <v>31.888888888888893</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>31.06666666666667</v>
+        <v>31.888888888888893</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,7 +1625,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>24.4</v>
+        <v>20.333333333333332</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1600,11 +1635,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>24.4</v>
+        <v>20.333333333333332</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>24.4</v>
+        <v>20.333333333333332</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,7 +1648,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>23.2</v>
+        <v>25.833333333333336</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1623,11 +1658,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>23.2</v>
+        <v>25.833333333333336</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>23.2</v>
+        <v>25.833333333333336</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1636,7 +1671,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>33.733333333333334</v>
+        <v>34.111111111111107</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1646,11 +1681,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>33.733333333333334</v>
+        <v>34.111111111111107</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>33.733333333333334</v>
+        <v>34.111111111111107</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1660,5 +1695,8 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F13" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Web 120 / Quiz 03
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79666CBD-AFC5-4B2E-B96E-9229729AACCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03686C28-8D97-4865-87B7-3B5FF5C89074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 120" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>No.</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>H06</t>
+  </si>
+  <si>
+    <t>Q03</t>
   </si>
 </sst>
 </file>
@@ -588,7 +591,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +603,7 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" customWidth="1"/>
@@ -630,7 +633,9 @@
       <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -664,7 +669,9 @@
       <c r="G2" s="15">
         <v>11</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="15">
+        <v>4.5</v>
+      </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -707,7 +714,9 @@
       <c r="G3" s="15">
         <v>10</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="15">
+        <v>8</v>
+      </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
@@ -750,7 +759,9 @@
       <c r="G4" s="15">
         <v>9.75</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="15">
+        <v>8.5</v>
+      </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -793,7 +804,9 @@
       <c r="G5" s="15">
         <v>8.5</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="15">
+        <v>5</v>
+      </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -836,7 +849,9 @@
       <c r="G6" s="15">
         <v>9.75</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="15">
+        <v>7.5</v>
+      </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -879,7 +894,9 @@
       <c r="G7" s="17">
         <v>9</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="17">
+        <v>8</v>
+      </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
@@ -921,7 +938,9 @@
       <c r="G8" s="17">
         <v>0</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
@@ -964,7 +983,9 @@
       <c r="G9" s="17">
         <v>10.5</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="17">
+        <v>8.5</v>
+      </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -1007,7 +1028,9 @@
       <c r="G10" s="17">
         <v>6.5</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="17">
+        <v>7</v>
+      </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1050,7 +1073,9 @@
       <c r="G11" s="17">
         <v>8</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="17">
+        <v>5</v>
+      </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
       <c r="K11" s="16"/>
@@ -1093,7 +1118,9 @@
       <c r="G12" s="17">
         <v>10.5</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="17">
+        <v>5.5</v>
+      </c>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
       <c r="K12" s="16"/>
@@ -1136,7 +1163,9 @@
       <c r="G13" s="17">
         <v>9</v>
       </c>
-      <c r="H13" s="16"/>
+      <c r="H13" s="17">
+        <v>8</v>
+      </c>
       <c r="I13" s="16"/>
       <c r="J13" s="17"/>
       <c r="K13" s="16"/>
@@ -1179,7 +1208,9 @@
       <c r="G14" s="17">
         <v>0</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="17">
+        <v>4.5</v>
+      </c>
       <c r="I14" s="16"/>
       <c r="J14" s="17"/>
       <c r="K14" s="16"/>
@@ -1222,7 +1253,9 @@
       <c r="G15" s="17">
         <v>9.75</v>
       </c>
-      <c r="H15" s="16"/>
+      <c r="H15" s="17">
+        <v>5.5</v>
+      </c>
       <c r="I15" s="16"/>
       <c r="J15" s="17"/>
       <c r="K15" s="16"/>
@@ -1265,7 +1298,9 @@
       <c r="G16" s="17">
         <v>9</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="17">
+        <v>6.5</v>
+      </c>
       <c r="I16" s="16"/>
       <c r="J16" s="17"/>
       <c r="K16" s="16"/>
@@ -1291,14 +1326,14 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
       <c r="K17" s="16"/>
@@ -1349,7 +1384,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>35.222222222222229</v>
+        <v>32.761904761904766</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1359,11 +1394,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>35.222222222222229</v>
+        <v>32.761904761904766</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>35.222222222222229</v>
+        <v>32.761904761904766</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1372,7 +1407,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>37.666666666666664</v>
+        <v>36.857142857142854</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1382,11 +1417,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>38.666666666666664</v>
+        <v>37.857142857142854</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>38.666666666666664</v>
+        <v>37.857142857142854</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1395,7 +1430,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>31.166666666666668</v>
+        <v>31.571428571428569</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1405,11 +1440,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>31.166666666666668</v>
+        <v>31.571428571428569</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>31.166666666666668</v>
+        <v>31.571428571428569</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1418,7 +1453,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>30.222222222222225</v>
+        <v>28.761904761904763</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1428,11 +1463,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>30.222222222222225</v>
+        <v>28.761904761904763</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>30.222222222222225</v>
+        <v>28.761904761904763</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1441,7 +1476,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>39</v>
+        <v>37.714285714285715</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1451,11 +1486,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>38.714285714285715</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38.714285714285715</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1464,7 +1499,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>35.777777777777771</v>
+        <v>35.238095238095241</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1474,11 +1509,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>35.777777777777771</v>
+        <v>35.238095238095241</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>35.777777777777771</v>
+        <v>35.238095238095241</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1510,7 +1545,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>38.166666666666671</v>
+        <v>37.571428571428569</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1520,11 +1555,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>39.166666666666671</v>
+        <v>38.571428571428569</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>39.166666666666671</v>
+        <v>38.571428571428569</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1533,7 +1568,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>30.777777777777775</v>
+        <v>30.38095238095238</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1543,11 +1578,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>30.777777777777775</v>
+        <v>30.38095238095238</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>30.777777777777775</v>
+        <v>30.38095238095238</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1556,7 +1591,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>28.111111111111107</v>
+        <v>26.952380952380949</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1566,11 +1601,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>29.111111111111107</v>
+        <v>27.952380952380949</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>29.111111111111107</v>
+        <v>27.952380952380949</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1579,7 +1614,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>33.666666666666664</v>
+        <v>32</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1589,11 +1624,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>33.666666666666664</v>
+        <v>32</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>33.666666666666664</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,7 +1637,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>31.888888888888893</v>
+        <v>31.904761904761905</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1612,11 +1647,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>31.888888888888893</v>
+        <v>31.904761904761905</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>31.888888888888893</v>
+        <v>31.904761904761905</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,7 +1660,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>20.333333333333332</v>
+        <v>20</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1635,11 +1670,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>20.333333333333332</v>
+        <v>20</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>20.333333333333332</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1648,7 +1683,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>25.833333333333336</v>
+        <v>25.285714285714285</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1658,11 +1693,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>25.833333333333336</v>
+        <v>25.285714285714285</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>25.833333333333336</v>
+        <v>25.285714285714285</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,7 +1706,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>34.111111111111107</v>
+        <v>32.952380952380949</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1681,11 +1716,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>34.111111111111107</v>
+        <v>32.952380952380949</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>34.111111111111107</v>
+        <v>32.952380952380949</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Homework 07
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03686C28-8D97-4865-87B7-3B5FF5C89074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AA713-6F2A-427A-949F-5F0147458018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2640" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 120" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Q03</t>
+  </si>
+  <si>
+    <t>H07</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +607,7 @@
     <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" customWidth="1"/>
     <col min="12" max="15" width="9.5703125" customWidth="1"/>
@@ -636,7 +639,9 @@
       <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -672,7 +677,9 @@
       <c r="H2" s="15">
         <v>4.5</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="15">
+        <v>9.5</v>
+      </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -717,7 +724,9 @@
       <c r="H3" s="15">
         <v>8</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="15">
+        <v>10</v>
+      </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
@@ -762,7 +771,9 @@
       <c r="H4" s="15">
         <v>8.5</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="15">
+        <v>9</v>
+      </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
@@ -807,7 +818,9 @@
       <c r="H5" s="15">
         <v>5</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="15">
+        <v>9</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -852,7 +865,9 @@
       <c r="H6" s="15">
         <v>7.5</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="15">
+        <v>10</v>
+      </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -897,7 +912,9 @@
       <c r="H7" s="17">
         <v>8</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="17">
+        <v>8.5</v>
+      </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
@@ -941,7 +958,9 @@
       <c r="H8" s="17">
         <v>0</v>
       </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
@@ -986,7 +1005,9 @@
       <c r="H9" s="17">
         <v>8.5</v>
       </c>
-      <c r="I9" s="17"/>
+      <c r="I9" s="17">
+        <v>9.5</v>
+      </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
@@ -1031,7 +1052,9 @@
       <c r="H10" s="17">
         <v>7</v>
       </c>
-      <c r="I10" s="17"/>
+      <c r="I10" s="17">
+        <v>8.5</v>
+      </c>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
@@ -1076,7 +1099,9 @@
       <c r="H11" s="17">
         <v>5</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="17">
+        <v>9.5</v>
+      </c>
       <c r="J11" s="17"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
@@ -1121,7 +1146,9 @@
       <c r="H12" s="17">
         <v>5.5</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="17">
+        <v>9.5</v>
+      </c>
       <c r="J12" s="17"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -1166,7 +1193,10 @@
       <c r="H13" s="17">
         <v>8</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="18">
+        <f>9.5/2</f>
+        <v>4.75</v>
+      </c>
       <c r="J13" s="17"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
@@ -1211,7 +1241,9 @@
       <c r="H14" s="17">
         <v>4.5</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="17">
+        <v>9</v>
+      </c>
       <c r="J14" s="17"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
@@ -1256,7 +1288,9 @@
       <c r="H15" s="17">
         <v>5.5</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="17">
+        <v>9.5</v>
+      </c>
       <c r="J15" s="17"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
@@ -1301,7 +1335,9 @@
       <c r="H16" s="17">
         <v>6.5</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="17">
+        <v>9.5</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
@@ -1326,7 +1362,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1334,7 +1370,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="16"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
@@ -1384,7 +1420,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>32.761904761904766</v>
+        <v>33.416666666666671</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1394,11 +1430,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>32.761904761904766</v>
+        <v>33.416666666666671</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>32.761904761904766</v>
+        <v>33.416666666666671</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1407,7 +1443,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>36.857142857142854</v>
+        <v>37.25</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1417,11 +1453,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>37.857142857142854</v>
+        <v>38.25</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>37.857142857142854</v>
+        <v>38.25</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1430,7 +1466,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>31.571428571428569</v>
+        <v>32.125</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1440,11 +1476,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>31.571428571428569</v>
+        <v>32.125</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>31.571428571428569</v>
+        <v>32.125</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1453,7 +1489,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>28.761904761904763</v>
+        <v>29.666666666666668</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1463,11 +1499,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>28.761904761904763</v>
+        <v>29.666666666666668</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>28.761904761904763</v>
+        <v>29.666666666666668</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1476,7 +1512,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>37.714285714285715</v>
+        <v>38</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1486,11 +1522,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>38.714285714285715</v>
+        <v>39</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>38.714285714285715</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1499,7 +1535,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>35.238095238095241</v>
+        <v>35.083333333333329</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1509,11 +1545,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>35.238095238095241</v>
+        <v>35.083333333333329</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>35.238095238095241</v>
+        <v>35.083333333333329</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1545,7 +1581,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>37.571428571428569</v>
+        <v>37.625</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1555,11 +1591,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>38.571428571428569</v>
+        <v>38.625</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>38.571428571428569</v>
+        <v>38.625</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1568,7 +1604,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>30.38095238095238</v>
+        <v>30.833333333333329</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1578,11 +1614,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>30.38095238095238</v>
+        <v>30.833333333333329</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>30.38095238095238</v>
+        <v>30.833333333333329</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1591,7 +1627,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>26.952380952380949</v>
+        <v>28.333333333333329</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1601,11 +1637,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>27.952380952380949</v>
+        <v>29.333333333333329</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>27.952380952380949</v>
+        <v>29.333333333333329</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1614,7 +1650,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>32</v>
+        <v>32.75</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1624,11 +1660,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>32.75</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>32.75</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,7 +1673,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>31.904761904761905</v>
+        <v>30.291666666666668</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1647,11 +1683,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>31.904761904761905</v>
+        <v>30.291666666666668</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>31.904761904761905</v>
+        <v>30.291666666666668</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1660,7 +1696,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1670,11 +1706,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,7 +1719,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>25.285714285714285</v>
+        <v>26.875</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1693,11 +1729,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>25.285714285714285</v>
+        <v>26.875</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>25.285714285714285</v>
+        <v>26.875</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1706,7 +1742,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>32.952380952380949</v>
+        <v>33.583333333333329</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1716,11 +1752,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>32.952380952380949</v>
+        <v>33.583333333333329</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>32.952380952380949</v>
+        <v>33.583333333333329</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Homework 08
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AA713-6F2A-427A-949F-5F0147458018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E6A739-48D9-4747-8F7B-4B47B1D0A044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>No.</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>H07</t>
+  </si>
+  <si>
+    <t>H08</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +645,9 @@
       <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -680,7 +685,9 @@
       <c r="I2" s="15">
         <v>9.5</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="15">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
@@ -727,7 +734,9 @@
       <c r="I3" s="15">
         <v>10</v>
       </c>
-      <c r="J3" s="15"/>
+      <c r="J3" s="15">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
@@ -774,7 +783,9 @@
       <c r="I4" s="15">
         <v>9</v>
       </c>
-      <c r="J4" s="15"/>
+      <c r="J4" s="15">
+        <v>9.4</v>
+      </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -821,7 +832,9 @@
       <c r="I5" s="15">
         <v>9</v>
       </c>
-      <c r="J5" s="15"/>
+      <c r="J5" s="15">
+        <v>9.1</v>
+      </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -868,7 +881,9 @@
       <c r="I6" s="15">
         <v>10</v>
       </c>
-      <c r="J6" s="15"/>
+      <c r="J6" s="15">
+        <v>10.7</v>
+      </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -915,7 +930,9 @@
       <c r="I7" s="17">
         <v>8.5</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17">
+        <v>57</v>
+      </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
@@ -961,7 +978,9 @@
       <c r="I8" s="17">
         <v>0</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="17">
+        <v>0</v>
+      </c>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
@@ -1008,7 +1027,9 @@
       <c r="I9" s="17">
         <v>9.5</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="17">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
@@ -1055,7 +1076,9 @@
       <c r="I10" s="17">
         <v>8.5</v>
       </c>
-      <c r="J10" s="17"/>
+      <c r="J10" s="17">
+        <v>8.6999999999999993</v>
+      </c>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
@@ -1102,7 +1125,9 @@
       <c r="I11" s="17">
         <v>9.5</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="17">
+        <v>6.8</v>
+      </c>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
@@ -1149,7 +1174,9 @@
       <c r="I12" s="17">
         <v>9.5</v>
       </c>
-      <c r="J12" s="17"/>
+      <c r="J12" s="17">
+        <v>10</v>
+      </c>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -1197,7 +1224,9 @@
         <f>9.5/2</f>
         <v>4.75</v>
       </c>
-      <c r="J13" s="17"/>
+      <c r="J13" s="17">
+        <v>0</v>
+      </c>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
@@ -1244,7 +1273,9 @@
       <c r="I14" s="17">
         <v>9</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -1291,7 +1322,9 @@
       <c r="I15" s="17">
         <v>9.5</v>
       </c>
-      <c r="J15" s="17"/>
+      <c r="J15" s="17">
+        <v>7.1</v>
+      </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -1338,7 +1371,9 @@
       <c r="I16" s="17">
         <v>9.5</v>
       </c>
-      <c r="J16" s="17"/>
+      <c r="J16" s="17">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -1362,7 +1397,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1420,7 +1455,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>33.416666666666671</v>
+        <v>34.014814814814819</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1430,11 +1465,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>33.416666666666671</v>
+        <v>34.014814814814819</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>33.416666666666671</v>
+        <v>34.014814814814819</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1443,7 +1478,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>37.25</v>
+        <v>37.422222222222224</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1453,11 +1488,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>38.25</v>
+        <v>38.422222222222224</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>38.25</v>
+        <v>38.422222222222224</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1466,7 +1501,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>32.125</v>
+        <v>32.733333333333334</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1476,11 +1511,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>32.125</v>
+        <v>32.733333333333334</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>32.125</v>
+        <v>32.733333333333334</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1489,7 +1524,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>29.666666666666668</v>
+        <v>30.414814814814815</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1499,11 +1534,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>29.666666666666668</v>
+        <v>30.414814814814815</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>29.666666666666668</v>
+        <v>30.414814814814815</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1512,7 +1547,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>38</v>
+        <v>38.533333333333331</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1522,11 +1557,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>39.533333333333331</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>39.533333333333331</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1535,7 +1570,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>35.083333333333329</v>
+        <v>56.518518518518512</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1545,11 +1580,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>35.083333333333329</v>
+        <v>56.518518518518512</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>35.083333333333329</v>
+        <v>56.518518518518512</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1581,7 +1616,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>37.625</v>
+        <v>37.755555555555553</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1591,11 +1626,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>38.625</v>
+        <v>38.755555555555553</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>38.625</v>
+        <v>38.755555555555553</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1604,7 +1639,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>30.833333333333329</v>
+        <v>31.274074074074072</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1614,11 +1649,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>30.833333333333329</v>
+        <v>31.274074074074072</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>30.833333333333329</v>
+        <v>31.274074074074072</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1627,7 +1662,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>28.333333333333329</v>
+        <v>28.207407407407405</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1637,11 +1672,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>29.333333333333329</v>
+        <v>29.207407407407405</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>29.333333333333329</v>
+        <v>29.207407407407405</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1650,7 +1685,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>32.75</v>
+        <v>33.555555555555557</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1660,11 +1695,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>32.75</v>
+        <v>33.555555555555557</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>32.75</v>
+        <v>33.555555555555557</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1673,7 +1708,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>30.291666666666668</v>
+        <v>26.925925925925927</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1683,11 +1718,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>30.291666666666668</v>
+        <v>26.925925925925927</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>30.291666666666668</v>
+        <v>26.925925925925927</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,7 +1731,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>22</v>
+        <v>19.555555555555554</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1706,11 +1741,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>19.555555555555554</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>19.555555555555554</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,7 +1754,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>26.875</v>
+        <v>27.044444444444444</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1729,11 +1764,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>26.875</v>
+        <v>27.044444444444444</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>26.875</v>
+        <v>27.044444444444444</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,7 +1777,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>33.583333333333329</v>
+        <v>33.762962962962959</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1752,11 +1787,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>33.583333333333329</v>
+        <v>33.762962962962959</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>33.583333333333329</v>
+        <v>33.762962962962959</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Quiz 04
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F65E0-359D-4B33-B9D3-2256333C6592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20018014-598F-4FC0-866F-AC7439A38D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>No.</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>H08</t>
+  </si>
+  <si>
+    <t>Q04</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +615,7 @@
     <col min="8" max="8" width="10.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" customWidth="1"/>
     <col min="12" max="15" width="9.5703125" customWidth="1"/>
     <col min="16" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
@@ -648,7 +651,9 @@
       <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -680,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="15">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="I2" s="15">
         <v>9.5</v>
@@ -688,7 +693,10 @@
       <c r="J2" s="15">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="15">
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
@@ -729,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="15">
         <v>10</v>
@@ -737,7 +745,10 @@
       <c r="J3" s="15">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K3" s="15"/>
+      <c r="K3" s="15">
+        <f>(9/17)*10</f>
+        <v>5.2941176470588234</v>
+      </c>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
@@ -778,7 +789,7 @@
         <v>9.75</v>
       </c>
       <c r="H4" s="15">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="I4" s="15">
         <v>9</v>
@@ -786,7 +797,10 @@
       <c r="J4" s="15">
         <v>9.4</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="15">
+        <f>(15/17)*10</f>
+        <v>8.8235294117647065</v>
+      </c>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
       <c r="N4" s="17"/>
@@ -827,7 +841,7 @@
         <v>8.5</v>
       </c>
       <c r="H5" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="15">
         <v>9</v>
@@ -835,7 +849,10 @@
       <c r="J5" s="15">
         <v>9.1</v>
       </c>
-      <c r="K5" s="15"/>
+      <c r="K5" s="15">
+        <f>(10/17)*10</f>
+        <v>5.882352941176471</v>
+      </c>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="17"/>
@@ -876,7 +893,7 @@
         <v>9.75</v>
       </c>
       <c r="H6" s="15">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="I6" s="15">
         <v>10</v>
@@ -884,7 +901,10 @@
       <c r="J6" s="15">
         <v>10.7</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="15">
+        <f>(10/17)*10</f>
+        <v>5.882352941176471</v>
+      </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="17"/>
@@ -925,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I7" s="17">
         <v>8.5</v>
@@ -933,7 +953,10 @@
       <c r="J7" s="17">
         <v>5.7</v>
       </c>
-      <c r="K7" s="17"/>
+      <c r="K7" s="17">
+        <f>(12/17)*10</f>
+        <v>7.0588235294117654</v>
+      </c>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -981,7 +1004,9 @@
       <c r="J8" s="17">
         <v>0</v>
       </c>
-      <c r="K8" s="17"/>
+      <c r="K8" s="17">
+        <v>0</v>
+      </c>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
@@ -1022,7 +1047,7 @@
         <v>10.5</v>
       </c>
       <c r="H9" s="17">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="I9" s="17">
         <v>9.5</v>
@@ -1030,7 +1055,10 @@
       <c r="J9" s="17">
         <v>9.6999999999999993</v>
       </c>
-      <c r="K9" s="17"/>
+      <c r="K9" s="17">
+        <f>(11/17)*10</f>
+        <v>6.4705882352941178</v>
+      </c>
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
@@ -1071,7 +1099,7 @@
         <v>6.5</v>
       </c>
       <c r="H10" s="17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10" s="17">
         <v>8.5</v>
@@ -1079,7 +1107,10 @@
       <c r="J10" s="17">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="17">
+        <f>(8/17)*10</f>
+        <v>4.7058823529411766</v>
+      </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
@@ -1120,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="H11" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11" s="17">
         <v>9.5</v>
@@ -1128,7 +1159,10 @@
       <c r="J11" s="17">
         <v>6.8</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="17">
+        <f>7/17*10</f>
+        <v>4.117647058823529</v>
+      </c>
       <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
@@ -1169,7 +1203,7 @@
         <v>10.5</v>
       </c>
       <c r="H12" s="17">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="I12" s="17">
         <v>9.5</v>
@@ -1177,7 +1211,10 @@
       <c r="J12" s="17">
         <v>10</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="17">
+        <f>10/17*10</f>
+        <v>5.882352941176471</v>
+      </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
@@ -1218,7 +1255,7 @@
         <v>9</v>
       </c>
       <c r="H13" s="17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I13" s="18">
         <f>9.5/2</f>
@@ -1227,7 +1264,10 @@
       <c r="J13" s="17">
         <v>0</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="17">
+        <f>11/17*10</f>
+        <v>6.4705882352941178</v>
+      </c>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
@@ -1268,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="17">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="I14" s="17">
         <v>9</v>
@@ -1276,7 +1316,10 @@
       <c r="J14" s="17">
         <v>0</v>
       </c>
-      <c r="K14" s="16"/>
+      <c r="K14" s="17">
+        <f>7/17*10</f>
+        <v>4.117647058823529</v>
+      </c>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
@@ -1317,7 +1360,7 @@
         <v>9.75</v>
       </c>
       <c r="H15" s="17">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="I15" s="17">
         <v>9.5</v>
@@ -1325,7 +1368,10 @@
       <c r="J15" s="17">
         <v>7.1</v>
       </c>
-      <c r="K15" s="16"/>
+      <c r="K15" s="17">
+        <f>10/17*10</f>
+        <v>5.882352941176471</v>
+      </c>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
@@ -1366,7 +1412,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="17">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="I16" s="17">
         <v>9.5</v>
@@ -1374,7 +1420,10 @@
       <c r="J16" s="17">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="17">
+        <f>5/17*10</f>
+        <v>2.9411764705882355</v>
+      </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
@@ -1397,7 +1446,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1407,7 +1456,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
-      <c r="K17" s="16"/>
+      <c r="K17" s="17"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
@@ -1455,7 +1504,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>34.014814814814819</v>
+        <v>33.601568627450987</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1465,11 +1514,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>34.014814814814819</v>
+        <v>33.601568627450987</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>34.014814814814819</v>
+        <v>33.601568627450987</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1478,7 +1527,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>37.422222222222224</v>
+        <v>36.197647058823527</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1488,11 +1537,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>38.422222222222224</v>
+        <v>37.197647058823527</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>38.422222222222224</v>
+        <v>37.197647058823527</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1501,7 +1550,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>32.733333333333334</v>
+        <v>33.389411764705883</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1511,11 +1560,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>32.733333333333334</v>
+        <v>33.389411764705883</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>32.733333333333334</v>
+        <v>33.389411764705883</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1524,7 +1573,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>30.414814814814815</v>
+        <v>30.12627450980392</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1534,11 +1583,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>30.414814814814815</v>
+        <v>30.12627450980392</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>30.414814814814815</v>
+        <v>30.12627450980392</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1547,7 +1596,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>38.533333333333331</v>
+        <v>37.432941176470592</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1557,11 +1606,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>39.533333333333331</v>
+        <v>38.432941176470592</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>39.533333333333331</v>
+        <v>38.432941176470592</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1570,7 +1619,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>33.718518518518515</v>
+        <v>33.570196078431366</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1580,11 +1629,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>33.718518518518515</v>
+        <v>33.570196078431366</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>33.718518518518515</v>
+        <v>33.570196078431366</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1616,7 +1665,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>37.755555555555553</v>
+        <v>36.968235294117648</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1626,11 +1675,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>38.755555555555553</v>
+        <v>37.968235294117648</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>38.755555555555553</v>
+        <v>37.968235294117648</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1639,7 +1688,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>31.274074074074072</v>
+        <v>30.429019607843134</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1649,11 +1698,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>31.274074074074072</v>
+        <v>30.429019607843134</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>31.274074074074072</v>
+        <v>30.429019607843134</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1662,7 +1711,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>28.207407407407405</v>
+        <v>27.433725490196082</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1672,11 +1721,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>29.207407407407405</v>
+        <v>28.433725490196082</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>29.207407407407405</v>
+        <v>28.433725490196082</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1685,7 +1734,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>33.555555555555557</v>
+        <v>32.952941176470588</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1695,11 +1744,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>33.555555555555557</v>
+        <v>32.952941176470588</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>33.555555555555557</v>
+        <v>32.952941176470588</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,7 +1757,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>26.925925925925927</v>
+        <v>27.221568627450985</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1718,11 +1767,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>26.925925925925927</v>
+        <v>27.221568627450985</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>26.925925925925927</v>
+        <v>27.221568627450985</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1731,7 +1780,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>19.555555555555554</v>
+        <v>19.647058823529409</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1741,11 +1790,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>19.555555555555554</v>
+        <v>19.647058823529409</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>19.555555555555554</v>
+        <v>19.647058823529409</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,7 +1803,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>27.044444444444444</v>
+        <v>27.092941176470589</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1764,11 +1813,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>27.044444444444444</v>
+        <v>27.092941176470589</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>27.044444444444444</v>
+        <v>27.092941176470589</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,7 +1826,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>33.762962962962959</v>
+        <v>31.963137254901955</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1787,11 +1836,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>33.762962962962959</v>
+        <v>31.963137254901955</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>33.762962962962959</v>
+        <v>31.963137254901955</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Quiz 05
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20018014-598F-4FC0-866F-AC7439A38D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8548598-6465-4A75-A50D-9D90F9E4F7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>No.</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Q04</t>
+  </si>
+  <si>
+    <t>Q5</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +657,9 @@
       <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -697,7 +702,9 @@
         <f>(11/17)*10</f>
         <v>6.4705882352941178</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="15">
+        <v>7.42</v>
+      </c>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
@@ -749,7 +756,9 @@
         <f>(9/17)*10</f>
         <v>5.2941176470588234</v>
       </c>
-      <c r="L3" s="15"/>
+      <c r="L3" s="15">
+        <v>8.85</v>
+      </c>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
@@ -801,7 +810,9 @@
         <f>(15/17)*10</f>
         <v>8.8235294117647065</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="15">
+        <v>8</v>
+      </c>
       <c r="M4" s="15"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
@@ -853,7 +864,9 @@
         <f>(10/17)*10</f>
         <v>5.882352941176471</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="15">
+        <v>6</v>
+      </c>
       <c r="M5" s="15"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
@@ -905,7 +918,9 @@
         <f>(10/17)*10</f>
         <v>5.882352941176471</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="15">
+        <v>9.14</v>
+      </c>
       <c r="M6" s="15"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
@@ -957,7 +972,9 @@
         <f>(12/17)*10</f>
         <v>7.0588235294117654</v>
       </c>
-      <c r="L7" s="17"/>
+      <c r="L7" s="17">
+        <v>9.42</v>
+      </c>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
@@ -1007,7 +1024,9 @@
       <c r="K8" s="17">
         <v>0</v>
       </c>
-      <c r="L8" s="17"/>
+      <c r="L8" s="17">
+        <v>0</v>
+      </c>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
@@ -1059,7 +1078,9 @@
         <f>(11/17)*10</f>
         <v>6.4705882352941178</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="17">
+        <v>9.14</v>
+      </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
@@ -1111,7 +1132,9 @@
         <f>(8/17)*10</f>
         <v>4.7058823529411766</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="17">
+        <v>9.42</v>
+      </c>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
@@ -1163,7 +1186,9 @@
         <f>7/17*10</f>
         <v>4.117647058823529</v>
       </c>
-      <c r="L11" s="16"/>
+      <c r="L11" s="17">
+        <v>7.42</v>
+      </c>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -1215,7 +1240,9 @@
         <f>10/17*10</f>
         <v>5.882352941176471</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="L12" s="17">
+        <v>9.42</v>
+      </c>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -1268,7 +1295,9 @@
         <f>11/17*10</f>
         <v>6.4705882352941178</v>
       </c>
-      <c r="L13" s="16"/>
+      <c r="L13" s="17">
+        <v>0</v>
+      </c>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
@@ -1320,7 +1349,9 @@
         <f>7/17*10</f>
         <v>4.117647058823529</v>
       </c>
-      <c r="L14" s="16"/>
+      <c r="L14" s="17">
+        <v>6.85</v>
+      </c>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
@@ -1372,7 +1403,9 @@
         <f>10/17*10</f>
         <v>5.882352941176471</v>
       </c>
-      <c r="L15" s="16"/>
+      <c r="L15" s="17">
+        <v>7.71</v>
+      </c>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
@@ -1424,7 +1457,9 @@
         <f>5/17*10</f>
         <v>2.9411764705882355</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="17">
+        <v>8.57</v>
+      </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -1446,7 +1481,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1504,7 +1539,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>33.601568627450987</v>
+        <v>33.245062388591805</v>
       </c>
       <c r="C22" s="9">
         <v>0</v>
@@ -1514,11 +1549,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>33.601568627450987</v>
+        <v>33.245062388591805</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>33.601568627450987</v>
+        <v>33.245062388591805</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1527,7 +1562,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>36.197647058823527</v>
+        <v>36.125133689839572</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1537,11 +1572,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>37.197647058823527</v>
+        <v>37.125133689839572</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>37.197647058823527</v>
+        <v>37.125133689839572</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1550,7 +1585,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>33.389411764705883</v>
+        <v>33.263101604278077</v>
       </c>
       <c r="C24" s="9">
         <v>0</v>
@@ -1560,11 +1595,11 @@
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>33.389411764705883</v>
+        <v>33.263101604278077</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>33.389411764705883</v>
+        <v>33.263101604278077</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1573,7 +1608,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>30.12627450980392</v>
+        <v>29.569340463458111</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1583,11 +1618,11 @@
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>30.12627450980392</v>
+        <v>29.569340463458111</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>30.12627450980392</v>
+        <v>29.569340463458111</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1596,7 +1631,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>37.432941176470592</v>
+        <v>37.35358288770054</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1606,11 +1641,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>38.432941176470592</v>
+        <v>38.35358288770054</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>38.432941176470592</v>
+        <v>38.35358288770054</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1619,7 +1654,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>33.570196078431366</v>
+        <v>33.943814616755795</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1629,11 +1664,11 @@
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>33.570196078431366</v>
+        <v>33.943814616755795</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>33.570196078431366</v>
+        <v>33.943814616755795</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1665,7 +1700,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>36.968235294117648</v>
+        <v>36.931122994652405</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1675,11 +1710,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>37.968235294117648</v>
+        <v>37.931122994652405</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>37.968235294117648</v>
+        <v>37.931122994652405</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1688,7 +1723,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>30.429019607843134</v>
+        <v>31.088199643493759</v>
       </c>
       <c r="C30" s="9">
         <v>0</v>
@@ -1698,11 +1733,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>30.429019607843134</v>
+        <v>31.088199643493759</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>30.429019607843134</v>
+        <v>31.088199643493759</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1711,7 +1746,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>27.433725490196082</v>
+        <v>27.637932263814623</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1721,11 +1756,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>28.433725490196082</v>
+        <v>28.637932263814623</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>28.433725490196082</v>
+        <v>28.637932263814623</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1734,7 +1769,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>32.952941176470588</v>
+        <v>33.382673796791444</v>
       </c>
       <c r="C32" s="9">
         <v>0</v>
@@ -1744,11 +1779,11 @@
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>32.952941176470588</v>
+        <v>33.382673796791444</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>32.952941176470588</v>
+        <v>33.382673796791444</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,7 +1792,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>27.221568627450985</v>
+        <v>24.746880570409985</v>
       </c>
       <c r="C33" s="9">
         <v>0</v>
@@ -1767,11 +1802,11 @@
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>27.221568627450985</v>
+        <v>24.746880570409985</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>27.221568627450985</v>
+        <v>24.746880570409985</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1780,7 +1815,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>19.647058823529409</v>
+        <v>20.35187165775401</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1790,11 +1825,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>19.647058823529409</v>
+        <v>20.35187165775401</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>19.647058823529409</v>
+        <v>20.35187165775401</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,7 +1838,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>27.092941176470589</v>
+        <v>27.433582887700535</v>
       </c>
       <c r="C35" s="9">
         <v>0</v>
@@ -1813,11 +1848,11 @@
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>27.092941176470589</v>
+        <v>27.433582887700535</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>27.092941176470589</v>
+        <v>27.433582887700535</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1826,7 +1861,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>31.963137254901955</v>
+        <v>32.173761140819963</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
@@ -1836,11 +1871,11 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>31.963137254901955</v>
+        <v>32.173761140819963</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>31.963137254901955</v>
+        <v>32.173761140819963</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Homework 10 & 11
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8548598-6465-4A75-A50D-9D90F9E4F7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD961C8-B382-4F42-AC5F-5DB932318808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>No.</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Q5</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
   </si>
 </sst>
 </file>
@@ -603,7 +609,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,8 +666,12 @@
       <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -705,8 +715,12 @@
       <c r="L2" s="15">
         <v>7.42</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
+      <c r="M2" s="15">
+        <v>10</v>
+      </c>
+      <c r="N2" s="15">
+        <v>10</v>
+      </c>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
@@ -759,8 +773,12 @@
       <c r="L3" s="15">
         <v>8.85</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
+      <c r="M3" s="15">
+        <v>10</v>
+      </c>
+      <c r="N3" s="15">
+        <v>9</v>
+      </c>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
@@ -813,8 +831,12 @@
       <c r="L4" s="15">
         <v>8</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="17"/>
+      <c r="M4" s="15">
+        <v>10</v>
+      </c>
+      <c r="N4" s="17">
+        <v>10</v>
+      </c>
       <c r="O4" s="17"/>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
@@ -867,8 +889,12 @@
       <c r="L5" s="15">
         <v>6</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="17"/>
+      <c r="M5" s="15">
+        <v>10</v>
+      </c>
+      <c r="N5" s="17">
+        <v>10</v>
+      </c>
       <c r="O5" s="17"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
@@ -921,8 +947,12 @@
       <c r="L6" s="15">
         <v>9.14</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="17"/>
+      <c r="M6" s="15">
+        <v>10</v>
+      </c>
+      <c r="N6" s="17">
+        <v>8.5</v>
+      </c>
       <c r="O6" s="17"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
@@ -975,8 +1005,12 @@
       <c r="L7" s="17">
         <v>9.42</v>
       </c>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
+      <c r="M7" s="17">
+        <v>9</v>
+      </c>
+      <c r="N7" s="17">
+        <v>9</v>
+      </c>
       <c r="O7" s="17"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
@@ -1027,8 +1061,12 @@
       <c r="L8" s="17">
         <v>0</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
+      <c r="M8" s="17">
+        <v>0</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
       <c r="O8" s="17"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
@@ -1081,8 +1119,12 @@
       <c r="L9" s="17">
         <v>9.14</v>
       </c>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
+      <c r="M9" s="17">
+        <v>10</v>
+      </c>
+      <c r="N9" s="17">
+        <v>10.5</v>
+      </c>
       <c r="O9" s="17"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
@@ -1135,8 +1177,12 @@
       <c r="L10" s="17">
         <v>9.42</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
+      <c r="M10" s="17">
+        <v>10</v>
+      </c>
+      <c r="N10" s="17">
+        <v>7</v>
+      </c>
       <c r="O10" s="17"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
@@ -1189,8 +1235,12 @@
       <c r="L11" s="17">
         <v>7.42</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
+      <c r="M11" s="17">
+        <v>10</v>
+      </c>
+      <c r="N11" s="17">
+        <v>8.5</v>
+      </c>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
@@ -1243,8 +1293,12 @@
       <c r="L12" s="17">
         <v>9.42</v>
       </c>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
+      <c r="M12" s="17">
+        <v>10</v>
+      </c>
+      <c r="N12" s="17">
+        <v>11</v>
+      </c>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
@@ -1298,8 +1352,12 @@
       <c r="L13" s="17">
         <v>0</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
+      <c r="M13" s="17">
+        <v>10</v>
+      </c>
+      <c r="N13" s="17">
+        <v>8.5</v>
+      </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="Q13" s="16"/>
@@ -1352,8 +1410,12 @@
       <c r="L14" s="17">
         <v>6.85</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
+      <c r="M14" s="17">
+        <v>10</v>
+      </c>
+      <c r="N14" s="17">
+        <v>5</v>
+      </c>
       <c r="O14" s="16"/>
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
@@ -1406,8 +1468,12 @@
       <c r="L15" s="17">
         <v>7.71</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
+      <c r="M15" s="17">
+        <v>10</v>
+      </c>
+      <c r="N15" s="17">
+        <v>8</v>
+      </c>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
@@ -1460,8 +1526,12 @@
       <c r="L16" s="17">
         <v>8.57</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
+      <c r="M16" s="17">
+        <v>10</v>
+      </c>
+      <c r="N16" s="17">
+        <v>8.5</v>
+      </c>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
@@ -1481,7 +1551,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1539,21 +1609,21 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>33.245062388591805</v>
+        <v>34.28428355957768</v>
       </c>
       <c r="C22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="9">
         <v>0</v>
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>33.245062388591805</v>
+        <v>35.28428355957768</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>33.245062388591805</v>
+        <v>35.28428355957768</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1562,7 +1632,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>36.125133689839572</v>
+        <v>36.413574660633486</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1572,11 +1642,11 @@
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>37.125133689839572</v>
+        <v>37.413574660633486</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>37.125133689839572</v>
+        <v>37.413574660633486</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1585,21 +1655,21 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>33.263101604278077</v>
+        <v>34.29954751131222</v>
       </c>
       <c r="C24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="9">
         <v>0</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" si="0"/>
-        <v>33.263101604278077</v>
+        <v>35.29954751131222</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="1"/>
-        <v>33.263101604278077</v>
+        <v>35.29954751131222</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1608,21 +1678,21 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>29.569340463458111</v>
+        <v>31.174057315233785</v>
       </c>
       <c r="C25" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="9">
         <v>0</v>
       </c>
       <c r="E25" s="10">
         <f t="shared" si="0"/>
-        <v>29.569340463458111</v>
+        <v>32.174057315233782</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="1"/>
-        <v>29.569340463458111</v>
+        <v>32.174057315233782</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1631,7 +1701,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>37.35358288770054</v>
+        <v>37.299185520361995</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1641,11 +1711,11 @@
       </c>
       <c r="E26" s="10">
         <f t="shared" si="0"/>
-        <v>38.35358288770054</v>
+        <v>38.299185520361995</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="1"/>
-        <v>38.35358288770054</v>
+        <v>38.299185520361995</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1654,21 +1724,21 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>33.943814616755795</v>
+        <v>34.260150829562591</v>
       </c>
       <c r="C27" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="9">
         <v>0</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" si="0"/>
-        <v>33.943814616755795</v>
+        <v>35.260150829562591</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="1"/>
-        <v>33.943814616755795</v>
+        <v>35.260150829562591</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1700,7 +1770,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>36.931122994652405</v>
+        <v>37.557104072398189</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1710,11 +1780,11 @@
       </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>37.931122994652405</v>
+        <v>38.557104072398189</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="1"/>
-        <v>37.931122994652405</v>
+        <v>38.557104072398189</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1723,21 +1793,21 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>31.088199643493759</v>
+        <v>31.536168929110104</v>
       </c>
       <c r="C30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="9">
         <v>0</v>
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>31.088199643493759</v>
+        <v>32.536168929110104</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>31.088199643493759</v>
+        <v>32.536168929110104</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1746,7 +1816,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>27.637932263814623</v>
+        <v>29.078250377073907</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1756,11 +1826,11 @@
       </c>
       <c r="E31" s="10">
         <f t="shared" si="0"/>
-        <v>28.637932263814623</v>
+        <v>30.078250377073907</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="1"/>
-        <v>28.637932263814623</v>
+        <v>30.078250377073907</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1769,21 +1839,21 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>33.382673796791444</v>
+        <v>34.708416289592762</v>
       </c>
       <c r="C32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="9">
         <v>0</v>
       </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>33.382673796791444</v>
+        <v>35.708416289592762</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="1"/>
-        <v>33.382673796791444</v>
+        <v>35.708416289592762</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1792,21 +1862,21 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>24.746880570409985</v>
+        <v>26.631975867269986</v>
       </c>
       <c r="C33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="9">
         <v>0</v>
       </c>
       <c r="E33" s="10">
         <f t="shared" si="0"/>
-        <v>24.746880570409985</v>
+        <v>27.631975867269986</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="1"/>
-        <v>24.746880570409985</v>
+        <v>27.631975867269986</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1815,7 +1885,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>20.35187165775401</v>
+        <v>21.836199095022625</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1825,11 +1895,11 @@
       </c>
       <c r="E34" s="10">
         <f t="shared" si="0"/>
-        <v>20.35187165775401</v>
+        <v>21.836199095022625</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="1"/>
-        <v>20.35187165775401</v>
+        <v>21.836199095022625</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,21 +1908,21 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>27.433582887700535</v>
+        <v>28.751493212669679</v>
       </c>
       <c r="C35" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="9">
         <v>0</v>
       </c>
       <c r="E35" s="10">
         <f t="shared" si="0"/>
-        <v>27.433582887700535</v>
+        <v>29.751493212669679</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="1"/>
-        <v>27.433582887700535</v>
+        <v>29.751493212669679</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1861,21 +1931,21 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>32.173761140819963</v>
+        <v>32.91625942684766</v>
       </c>
       <c r="C36" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="9">
         <v>0</v>
       </c>
       <c r="E36" s="10">
         <f t="shared" si="0"/>
-        <v>32.173761140819963</v>
+        <v>33.91625942684766</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>32.173761140819963</v>
+        <v>33.91625942684766</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
web 120 / Homework 14
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD961C8-B382-4F42-AC5F-5DB932318808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE694C7-FD93-4C82-9402-89C28C0197D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>No.</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>H11</t>
+  </si>
+  <si>
+    <t>H14</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +675,9 @@
       <c r="N1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
@@ -721,7 +726,10 @@
       <c r="N2" s="15">
         <v>10</v>
       </c>
-      <c r="O2" s="15"/>
+      <c r="O2" s="15">
+        <f>(40/40)*10</f>
+        <v>10</v>
+      </c>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="16"/>
@@ -779,7 +787,10 @@
       <c r="N3" s="15">
         <v>9</v>
       </c>
-      <c r="O3" s="15"/>
+      <c r="O3" s="15">
+        <f t="shared" ref="O3:O16" si="0">(40/40)*10</f>
+        <v>10</v>
+      </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="16"/>
@@ -837,7 +848,10 @@
       <c r="N4" s="17">
         <v>10</v>
       </c>
-      <c r="O4" s="17"/>
+      <c r="O4" s="15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
@@ -895,7 +909,10 @@
       <c r="N5" s="17">
         <v>10</v>
       </c>
-      <c r="O5" s="17"/>
+      <c r="O5" s="15">
+        <f>(38/40)*10</f>
+        <v>9.5</v>
+      </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -953,7 +970,9 @@
       <c r="N6" s="17">
         <v>8.5</v>
       </c>
-      <c r="O6" s="17"/>
+      <c r="O6" s="15">
+        <v>0</v>
+      </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
@@ -1011,7 +1030,10 @@
       <c r="N7" s="17">
         <v>9</v>
       </c>
-      <c r="O7" s="17"/>
+      <c r="O7" s="15">
+        <f>(38/40)*10</f>
+        <v>9.5</v>
+      </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
@@ -1067,7 +1089,9 @@
       <c r="N8" s="17">
         <v>0</v>
       </c>
-      <c r="O8" s="17"/>
+      <c r="O8" s="15">
+        <v>0</v>
+      </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
@@ -1125,7 +1149,10 @@
       <c r="N9" s="17">
         <v>10.5</v>
       </c>
-      <c r="O9" s="17"/>
+      <c r="O9" s="15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
@@ -1183,7 +1210,10 @@
       <c r="N10" s="17">
         <v>7</v>
       </c>
-      <c r="O10" s="17"/>
+      <c r="O10" s="15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
@@ -1241,7 +1271,10 @@
       <c r="N11" s="17">
         <v>8.5</v>
       </c>
-      <c r="O11" s="16"/>
+      <c r="O11" s="15">
+        <f>(39/40)*10</f>
+        <v>9.75</v>
+      </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
@@ -1299,7 +1332,10 @@
       <c r="N12" s="17">
         <v>11</v>
       </c>
-      <c r="O12" s="16"/>
+      <c r="O12" s="15">
+        <f>(39/40)*10</f>
+        <v>9.75</v>
+      </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
@@ -1358,7 +1394,9 @@
       <c r="N13" s="17">
         <v>8.5</v>
       </c>
-      <c r="O13" s="16"/>
+      <c r="O13" s="15">
+        <v>0</v>
+      </c>
       <c r="P13" s="16"/>
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
@@ -1416,7 +1454,9 @@
       <c r="N14" s="17">
         <v>5</v>
       </c>
-      <c r="O14" s="16"/>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
@@ -1474,7 +1514,10 @@
       <c r="N15" s="17">
         <v>8</v>
       </c>
-      <c r="O15" s="16"/>
+      <c r="O15" s="15">
+        <f>(38/40)*10</f>
+        <v>9.5</v>
+      </c>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
@@ -1532,7 +1575,10 @@
       <c r="N16" s="17">
         <v>8.5</v>
       </c>
-      <c r="O16" s="16"/>
+      <c r="O16" s="15">
+        <f>(39/40)*10</f>
+        <v>9.75</v>
+      </c>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
@@ -1551,7 +1597,7 @@
       </c>
       <c r="B17" s="5">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1609,7 +1655,7 @@
       </c>
       <c r="B22" s="8">
         <f>(SUM(B2:R2)/B17) * 40</f>
-        <v>34.28428355957768</v>
+        <v>34.692549019607846</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
@@ -1619,11 +1665,11 @@
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>35.28428355957768</v>
+        <v>35.692549019607846</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>35.28428355957768</v>
+        <v>35.692549019607846</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1632,7 +1678,7 @@
       </c>
       <c r="B23" s="8">
         <f>(SUM(B3:R3)/B17) * 40</f>
-        <v>36.413574660633486</v>
+        <v>36.669747899159667</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1641,12 +1687,12 @@
         <v>0</v>
       </c>
       <c r="E23" s="10">
-        <f t="shared" ref="E23:E36" si="0">B23+C23+D23</f>
-        <v>37.413574660633486</v>
+        <f t="shared" ref="E23:E36" si="1">B23+C23+D23</f>
+        <v>37.669747899159667</v>
       </c>
       <c r="F23" s="12">
-        <f t="shared" ref="F23:F36" si="1">E23</f>
-        <v>37.413574660633486</v>
+        <f t="shared" ref="F23:F36" si="2">E23</f>
+        <v>37.669747899159667</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1655,7 +1701,7 @@
       </c>
       <c r="B24" s="8">
         <f>(SUM(B4:R4)/B17) * 40</f>
-        <v>34.29954751131222</v>
+        <v>34.706722689075633</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -1664,12 +1710,12 @@
         <v>0</v>
       </c>
       <c r="E24" s="10">
-        <f t="shared" si="0"/>
-        <v>35.29954751131222</v>
+        <f t="shared" si="1"/>
+        <v>35.706722689075633</v>
       </c>
       <c r="F24" s="12">
-        <f t="shared" si="1"/>
-        <v>35.29954751131222</v>
+        <f t="shared" si="2"/>
+        <v>35.706722689075633</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1678,7 +1724,7 @@
       </c>
       <c r="B25" s="8">
         <f>(SUM(B5:R5)/B17) * 40</f>
-        <v>31.174057315233785</v>
+        <v>31.661624649859945</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
@@ -1687,12 +1733,12 @@
         <v>0</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="0"/>
-        <v>32.174057315233782</v>
+        <f t="shared" si="1"/>
+        <v>32.661624649859945</v>
       </c>
       <c r="F25" s="12">
-        <f t="shared" si="1"/>
-        <v>32.174057315233782</v>
+        <f t="shared" si="2"/>
+        <v>32.661624649859945</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1701,7 +1747,7 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>37.299185520361995</v>
+        <v>34.634957983193281</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -1710,12 +1756,12 @@
         <v>0</v>
       </c>
       <c r="E26" s="10">
-        <f t="shared" si="0"/>
-        <v>38.299185520361995</v>
+        <f t="shared" si="1"/>
+        <v>35.634957983193281</v>
       </c>
       <c r="F26" s="12">
-        <f t="shared" si="1"/>
-        <v>38.299185520361995</v>
+        <f t="shared" si="2"/>
+        <v>35.634957983193281</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1724,7 +1770,7 @@
       </c>
       <c r="B27" s="8">
         <f>(SUM(B7:R7)/B17) * 40</f>
-        <v>34.260150829562591</v>
+        <v>34.527282913165266</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
@@ -1733,12 +1779,12 @@
         <v>0</v>
       </c>
       <c r="E27" s="10">
-        <f t="shared" si="0"/>
-        <v>35.260150829562591</v>
+        <f t="shared" si="1"/>
+        <v>35.527282913165266</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="1"/>
-        <v>35.260150829562591</v>
+        <f t="shared" si="2"/>
+        <v>35.527282913165266</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1756,11 +1802,11 @@
         <v>0</v>
       </c>
       <c r="E28" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F28" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1770,7 +1816,7 @@
       </c>
       <c r="B29" s="8">
         <f>(SUM(B9:R9)/B17) * 40</f>
-        <v>37.557104072398189</v>
+        <v>37.731596638655461</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -1779,12 +1825,12 @@
         <v>0</v>
       </c>
       <c r="E29" s="10">
-        <f t="shared" si="0"/>
-        <v>38.557104072398189</v>
+        <f t="shared" si="1"/>
+        <v>38.731596638655461</v>
       </c>
       <c r="F29" s="12">
-        <f t="shared" si="1"/>
-        <v>38.557104072398189</v>
+        <f t="shared" si="2"/>
+        <v>38.731596638655461</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1793,7 +1839,7 @@
       </c>
       <c r="B30" s="8">
         <f>(SUM(B10:R10)/B17) * 40</f>
-        <v>31.536168929110104</v>
+        <v>32.140728291316528</v>
       </c>
       <c r="C30" s="9">
         <v>1</v>
@@ -1803,11 +1849,11 @@
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>32.536168929110104</v>
+        <v>33.140728291316528</v>
       </c>
       <c r="F30" s="12">
-        <f t="shared" si="1"/>
-        <v>32.536168929110104</v>
+        <f t="shared" si="2"/>
+        <v>33.140728291316528</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1816,7 +1862,7 @@
       </c>
       <c r="B31" s="8">
         <f>(SUM(B11:R11)/B17) * 40</f>
-        <v>29.078250377073907</v>
+        <v>29.786946778711489</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -1825,12 +1871,12 @@
         <v>0</v>
       </c>
       <c r="E31" s="10">
-        <f t="shared" si="0"/>
-        <v>30.078250377073907</v>
+        <f t="shared" si="1"/>
+        <v>30.786946778711489</v>
       </c>
       <c r="F31" s="12">
-        <f t="shared" si="1"/>
-        <v>30.078250377073907</v>
+        <f t="shared" si="2"/>
+        <v>30.786946778711489</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1839,7 +1885,7 @@
       </c>
       <c r="B32" s="8">
         <f>(SUM(B12:R12)/B17) * 40</f>
-        <v>34.708416289592762</v>
+        <v>35.014957983193277</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -1848,12 +1894,12 @@
         <v>0</v>
       </c>
       <c r="E32" s="10">
-        <f t="shared" si="0"/>
-        <v>35.708416289592762</v>
+        <f t="shared" si="1"/>
+        <v>36.014957983193277</v>
       </c>
       <c r="F32" s="12">
-        <f t="shared" si="1"/>
-        <v>35.708416289592762</v>
+        <f t="shared" si="2"/>
+        <v>36.014957983193277</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1862,7 +1908,7 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>26.631975867269986</v>
+        <v>24.729691876750699</v>
       </c>
       <c r="C33" s="9">
         <v>1</v>
@@ -1871,12 +1917,12 @@
         <v>0</v>
       </c>
       <c r="E33" s="10">
-        <f t="shared" si="0"/>
-        <v>27.631975867269986</v>
+        <f t="shared" si="1"/>
+        <v>25.729691876750699</v>
       </c>
       <c r="F33" s="12">
-        <f t="shared" si="1"/>
-        <v>27.631975867269986</v>
+        <f t="shared" si="2"/>
+        <v>25.729691876750699</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,7 +1931,7 @@
       </c>
       <c r="B34" s="8">
         <f>(SUM(B14:R14)/B17) * 40</f>
-        <v>21.836199095022625</v>
+        <v>20.276470588235295</v>
       </c>
       <c r="C34" s="9">
         <v>0</v>
@@ -1894,12 +1940,12 @@
         <v>0</v>
       </c>
       <c r="E34" s="10">
-        <f t="shared" si="0"/>
-        <v>21.836199095022625</v>
+        <f t="shared" si="1"/>
+        <v>20.276470588235295</v>
       </c>
       <c r="F34" s="12">
-        <f t="shared" si="1"/>
-        <v>21.836199095022625</v>
+        <f t="shared" si="2"/>
+        <v>20.276470588235295</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,7 +1954,7 @@
       </c>
       <c r="B35" s="8">
         <f>(SUM(B15:R15)/B17) * 40</f>
-        <v>28.751493212669679</v>
+        <v>29.412100840336134</v>
       </c>
       <c r="C35" s="9">
         <v>1</v>
@@ -1917,12 +1963,12 @@
         <v>0</v>
       </c>
       <c r="E35" s="10">
-        <f t="shared" si="0"/>
-        <v>29.751493212669679</v>
+        <f t="shared" si="1"/>
+        <v>30.412100840336134</v>
       </c>
       <c r="F35" s="12">
-        <f t="shared" si="1"/>
-        <v>29.751493212669679</v>
+        <f t="shared" si="2"/>
+        <v>30.412100840336134</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,7 +1977,7 @@
       </c>
       <c r="B36" s="8">
         <f>(SUM(B16:R16)/B17) * 40</f>
-        <v>32.91625942684766</v>
+        <v>33.350812324929969</v>
       </c>
       <c r="C36" s="9">
         <v>1</v>
@@ -1940,12 +1986,12 @@
         <v>0</v>
       </c>
       <c r="E36" s="10">
-        <f t="shared" si="0"/>
-        <v>33.91625942684766</v>
+        <f t="shared" si="1"/>
+        <v>34.350812324929969</v>
       </c>
       <c r="F36" s="12">
-        <f t="shared" si="1"/>
-        <v>33.91625942684766</v>
+        <f t="shared" si="2"/>
+        <v>34.350812324929969</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Scores updated
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE694C7-FD93-4C82-9402-89C28C0197D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A4C55-BE3C-4928-9559-54C5D3DE0838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
         <v>9</v>
       </c>
       <c r="O3" s="15">
-        <f t="shared" ref="O3:O16" si="0">(40/40)*10</f>
+        <f t="shared" ref="O3:O10" si="0">(40/40)*10</f>
         <v>10</v>
       </c>
       <c r="P3" s="15"/>
@@ -971,7 +971,7 @@
         <v>8.5</v>
       </c>
       <c r="O6" s="15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
@@ -1374,9 +1374,9 @@
       <c r="H13" s="17">
         <v>9</v>
       </c>
-      <c r="I13" s="18">
-        <f>9.5/2</f>
-        <v>4.75</v>
+      <c r="I13" s="15">
+        <f>9.5</f>
+        <v>9.5</v>
       </c>
       <c r="J13" s="17">
         <v>0</v>
@@ -1658,18 +1658,18 @@
         <v>34.692549019607846</v>
       </c>
       <c r="C22" s="9">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D22" s="9">
         <v>0</v>
       </c>
       <c r="E22" s="10">
         <f>B22+C22+D22</f>
-        <v>35.692549019607846</v>
+        <v>44.192549019607846</v>
       </c>
       <c r="F22" s="12">
         <f>E22</f>
-        <v>35.692549019607846</v>
+        <v>44.192549019607846</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1681,18 +1681,18 @@
         <v>36.669747899159667</v>
       </c>
       <c r="C23" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D23" s="9">
         <v>0</v>
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E36" si="1">B23+C23+D23</f>
-        <v>37.669747899159667</v>
+        <v>46.669747899159667</v>
       </c>
       <c r="F23" s="12">
         <f t="shared" ref="F23:F36" si="2">E23</f>
-        <v>37.669747899159667</v>
+        <v>46.669747899159667</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1704,18 +1704,18 @@
         <v>34.706722689075633</v>
       </c>
       <c r="C24" s="9">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D24" s="9">
         <v>0</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" si="1"/>
-        <v>35.706722689075633</v>
+        <v>44.206722689075633</v>
       </c>
       <c r="F24" s="12">
         <f t="shared" si="2"/>
-        <v>35.706722689075633</v>
+        <v>44.206722689075633</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1727,18 +1727,18 @@
         <v>31.661624649859945</v>
       </c>
       <c r="C25" s="9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D25" s="9">
         <v>0</v>
       </c>
       <c r="E25" s="10">
         <f t="shared" si="1"/>
-        <v>32.661624649859945</v>
+        <v>40.661624649859945</v>
       </c>
       <c r="F25" s="12">
         <f t="shared" si="2"/>
-        <v>32.661624649859945</v>
+        <v>40.661624649859945</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1747,21 +1747,21 @@
       </c>
       <c r="B26" s="8">
         <f>(SUM(B6:R6)/B17) * 40</f>
-        <v>34.634957983193281</v>
+        <v>37.492100840336143</v>
       </c>
       <c r="C26" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D26" s="9">
         <v>0</v>
       </c>
       <c r="E26" s="10">
         <f t="shared" si="1"/>
-        <v>35.634957983193281</v>
+        <v>47.492100840336143</v>
       </c>
       <c r="F26" s="12">
         <f t="shared" si="2"/>
-        <v>35.634957983193281</v>
+        <v>47.492100840336143</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1773,18 +1773,18 @@
         <v>34.527282913165266</v>
       </c>
       <c r="C27" s="9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D27" s="9">
         <v>0</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" si="1"/>
-        <v>35.527282913165266</v>
+        <v>43.527282913165266</v>
       </c>
       <c r="F27" s="12">
         <f t="shared" si="2"/>
-        <v>35.527282913165266</v>
+        <v>43.527282913165266</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1819,18 +1819,18 @@
         <v>37.731596638655461</v>
       </c>
       <c r="C29" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" s="9">
         <v>0</v>
       </c>
       <c r="E29" s="10">
         <f t="shared" si="1"/>
-        <v>38.731596638655461</v>
+        <v>47.731596638655461</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="2"/>
-        <v>38.731596638655461</v>
+        <v>47.731596638655461</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -1842,18 +1842,18 @@
         <v>32.140728291316528</v>
       </c>
       <c r="C30" s="9">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D30" s="9">
         <v>0</v>
       </c>
       <c r="E30" s="10">
         <f>B30+C30+D30</f>
-        <v>33.140728291316528</v>
+        <v>41.640728291316528</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="2"/>
-        <v>33.140728291316528</v>
+        <v>41.640728291316528</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1865,18 +1865,18 @@
         <v>29.786946778711489</v>
       </c>
       <c r="C31" s="9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D31" s="9">
         <v>0</v>
       </c>
       <c r="E31" s="10">
         <f t="shared" si="1"/>
-        <v>30.786946778711489</v>
+        <v>38.786946778711489</v>
       </c>
       <c r="F31" s="12">
         <f t="shared" si="2"/>
-        <v>30.786946778711489</v>
+        <v>38.786946778711489</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1888,18 +1888,18 @@
         <v>35.014957983193277</v>
       </c>
       <c r="C32" s="9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D32" s="9">
         <v>0</v>
       </c>
       <c r="E32" s="10">
         <f t="shared" si="1"/>
-        <v>36.014957983193277</v>
+        <v>45.014957983193277</v>
       </c>
       <c r="F32" s="12">
         <f t="shared" si="2"/>
-        <v>36.014957983193277</v>
+        <v>45.014957983193277</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,21 +1908,21 @@
       </c>
       <c r="B33" s="8">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>24.729691876750699</v>
+        <v>26.086834733893557</v>
       </c>
       <c r="C33" s="9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D33" s="9">
         <v>0</v>
       </c>
       <c r="E33" s="10">
         <f t="shared" si="1"/>
-        <v>25.729691876750699</v>
+        <v>34.086834733893554</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" si="2"/>
-        <v>25.729691876750699</v>
+        <v>34.086834733893554</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1934,18 +1934,18 @@
         <v>20.276470588235295</v>
       </c>
       <c r="C34" s="9">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="D34" s="9">
         <v>0</v>
       </c>
       <c r="E34" s="10">
         <f t="shared" si="1"/>
-        <v>20.276470588235295</v>
+        <v>28.776470588235295</v>
       </c>
       <c r="F34" s="12">
         <f t="shared" si="2"/>
-        <v>20.276470588235295</v>
+        <v>28.776470588235295</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,18 +1957,18 @@
         <v>29.412100840336134</v>
       </c>
       <c r="C35" s="9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D35" s="9">
         <v>0</v>
       </c>
       <c r="E35" s="10">
         <f t="shared" si="1"/>
-        <v>30.412100840336134</v>
+        <v>38.412100840336137</v>
       </c>
       <c r="F35" s="12">
         <f t="shared" si="2"/>
-        <v>30.412100840336134</v>
+        <v>38.412100840336137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1980,18 +1980,18 @@
         <v>33.350812324929969</v>
       </c>
       <c r="C36" s="9">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="D36" s="9">
         <v>0</v>
       </c>
       <c r="E36" s="10">
         <f t="shared" si="1"/>
-        <v>34.350812324929969</v>
+        <v>42.850812324929969</v>
       </c>
       <c r="F36" s="12">
         <f t="shared" si="2"/>
-        <v>34.350812324929969</v>
+        <v>42.850812324929969</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Final Project
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EE82EC-1DB7-44C0-802E-9F1EA6ED88CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1FAED3-9827-412C-842C-B3CA37C44C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,15 +1944,15 @@
         <v>9</v>
       </c>
       <c r="D35" s="15">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E35" s="16">
         <f t="shared" si="0"/>
-        <v>83.412100840336137</v>
+        <v>88.412100840336137</v>
       </c>
       <c r="F35" s="17">
         <f t="shared" si="1"/>
-        <v>83.412100840336137</v>
+        <v>88.412100840336137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Web 120 / Final Scores
</commit_message>
<xml_diff>
--- a/120/120.xlsx
+++ b/120/120.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\120\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37C9DE-395C-4B4D-A833-2C24B41AADDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAEABCC-3E40-454F-BCD2-391BEDE5E257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,13 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -597,7 +604,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1386,8 @@
         <v>8.5</v>
       </c>
       <c r="O13" s="4">
-        <v>0</v>
+        <f>(40/40)*10</f>
+        <v>10</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
@@ -1691,15 +1699,15 @@
         <v>9.5</v>
       </c>
       <c r="D24" s="15">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E24" s="16">
         <f t="shared" si="1"/>
-        <v>44.206722689075633</v>
+        <v>99.206722689075633</v>
       </c>
       <c r="F24" s="17">
         <f t="shared" si="0"/>
-        <v>44.206722689075633</v>
+        <v>99.206722689075633</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1714,15 +1722,15 @@
         <v>9</v>
       </c>
       <c r="D25" s="15">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E25" s="16">
         <f t="shared" si="1"/>
-        <v>40.661624649859945</v>
+        <v>90.661624649859945</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" si="0"/>
-        <v>40.661624649859945</v>
+        <v>90.661624649859945</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1737,15 +1745,15 @@
         <v>10</v>
       </c>
       <c r="D26" s="15">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E26" s="16">
         <f t="shared" si="1"/>
-        <v>47.492100840336143</v>
+        <v>107.49210084033615</v>
       </c>
       <c r="F26" s="17">
         <f t="shared" si="0"/>
-        <v>47.492100840336143</v>
+        <v>107.49210084033615</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1760,15 +1768,15 @@
         <v>9</v>
       </c>
       <c r="D27" s="15">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E27" s="16">
         <f t="shared" si="1"/>
-        <v>93.527282913165266</v>
+        <v>95.527282913165266</v>
       </c>
       <c r="F27" s="17">
         <f t="shared" si="0"/>
-        <v>93.527282913165266</v>
+        <v>95.527282913165266</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1852,15 +1860,15 @@
         <v>9</v>
       </c>
       <c r="D31" s="15">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E31" s="16">
         <f t="shared" si="1"/>
-        <v>68.786946778711496</v>
+        <v>70.786946778711496</v>
       </c>
       <c r="F31" s="17">
         <f t="shared" si="0"/>
-        <v>68.786946778711496</v>
+        <v>70.786946778711496</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1875,15 +1883,15 @@
         <v>10</v>
       </c>
       <c r="D32" s="15">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E32" s="16">
         <f t="shared" si="1"/>
-        <v>45.014957983193277</v>
+        <v>100.01495798319328</v>
       </c>
       <c r="F32" s="17">
         <f t="shared" si="0"/>
-        <v>45.014957983193277</v>
+        <v>100.01495798319328</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1892,21 +1900,21 @@
       </c>
       <c r="B33" s="14">
         <f>(SUM(B13:R13)/B17) * 40</f>
-        <v>26.086834733893557</v>
+        <v>28.943977591036418</v>
       </c>
       <c r="C33" s="15">
         <v>8</v>
       </c>
       <c r="D33" s="15">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E33" s="16">
         <f t="shared" si="1"/>
-        <v>34.086834733893554</v>
+        <v>86.943977591036415</v>
       </c>
       <c r="F33" s="17">
         <f t="shared" si="0"/>
-        <v>34.086834733893554</v>
+        <v>86.943977591036415</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,15 +1975,15 @@
         <v>9.5</v>
       </c>
       <c r="D36" s="15">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E36" s="16">
         <f t="shared" si="1"/>
-        <v>42.850812324929969</v>
+        <v>97.850812324929962</v>
       </c>
       <c r="F36" s="17">
         <f t="shared" si="0"/>
-        <v>42.850812324929969</v>
+        <v>97.850812324929962</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>